<commit_message>
Implemented several high-level optimizations
Implemented quadtree for tank-tank collision(not worth it!), made glow
per-tank instead of per-pixel on the screen (helps a lot!) and replaced
the free-bullet loop with an integer counting from 0 to MAXBULLET giving
most probably available bullets without looping.
</commit_message>
<xml_diff>
--- a/Report/PR3 Measurements.xlsx
+++ b/Report/PR3 Measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26775" windowHeight="13290"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="9000" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Measurements for PR3 Final Assignment</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Tweaking the backdrop line isn't worth it at all.</t>
+  </si>
+  <si>
+    <t>Update Tanks (Worst)</t>
+  </si>
+  <si>
+    <t>Update Tanks (Best)</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -803,6 +809,45 @@
     <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.75">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30">
+      <c r="B36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>18324819</v>
+      </c>
+      <c r="D37">
+        <v>19241248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>18324819</v>
+      </c>
+      <c r="D38">
+        <v>8215824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted optimizations to do better timings
</commit_message>
<xml_diff>
--- a/Report/PR3 Measurements.xlsx
+++ b/Report/PR3 Measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t>Measurements for PR3 Final Assignment</t>
   </si>
@@ -54,9 +54,6 @@
     <t xml:space="preserve"> - The rest</t>
   </si>
   <si>
-    <t>6 samples per measurement, for averages.</t>
-  </si>
-  <si>
     <t>Avg. FPS</t>
   </si>
   <si>
@@ -70,6 +67,21 @@
   </si>
   <si>
     <t>Update Tanks (Best)</t>
+  </si>
+  <si>
+    <t>QuadTree test</t>
+  </si>
+  <si>
+    <t>Only scaled "decently" above MAXP1=256</t>
+  </si>
+  <si>
+    <t>Smoke::Tick()</t>
+  </si>
+  <si>
+    <t>Identical values in columns means nothing was optimized in that stage</t>
+  </si>
+  <si>
+    <t>Smoke::Tick is per instance</t>
   </si>
 </sst>
 </file>
@@ -158,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -177,6 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -471,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,64 +511,59 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="28.5" customHeight="1">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8">
-        <v>94738</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9">
-        <v>106594007</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="B6" s="8">
+        <v>94738</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <v>72445</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="9">
-        <v>106416587</v>
+        <v>106594007</v>
+      </c>
+      <c r="D7">
+        <v>542734</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -564,10 +572,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="9">
-        <v>151212</v>
+        <v>106416587</v>
+      </c>
+      <c r="D8">
+        <v>356782</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -576,75 +587,83 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="11">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9">
+        <v>151212</v>
+      </c>
+      <c r="D9">
+        <v>159214</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="11">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="18.75">
-      <c r="A11" s="1" t="s">
+      <c r="D10">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75">
+      <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:9" ht="30">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
+      <c r="G13" s="3"/>
+      <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="8">
-        <v>281584</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="9">
-        <v>190303329</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="B14" s="8">
+        <v>281584</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
+        <v>254867</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="9">
-        <v>190003775</v>
-      </c>
-      <c r="D15" s="10"/>
+        <v>190303329</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1035457</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -653,12 +672,14 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="9">
-        <v>274187</v>
-      </c>
-      <c r="D16" s="10"/>
+        <v>190003775</v>
+      </c>
+      <c r="D16" s="10">
+        <v>690674</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -667,75 +688,84 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="9">
+        <v>274187</v>
+      </c>
+      <c r="D17" s="10">
+        <v>320689</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="18.75">
-      <c r="A19" s="1" t="s">
+      <c r="D18" s="10">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18.75">
+      <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
+    <row r="21" spans="1:9" ht="30">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4" t="s">
+      <c r="G21" s="3"/>
+      <c r="H21" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="8">
-        <v>3814491</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="9">
-        <v>606472930</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="B22" s="8">
+        <v>3814491</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6">
+        <v>3083085</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="9">
-        <v>606076953</v>
+        <v>606472930</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7">
+        <v>3324975</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -743,13 +773,15 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="9">
-        <v>371111</v>
+        <v>606076953</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7">
+        <v>2462142</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -757,24 +789,46 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="9">
-        <v>3</v>
+        <v>371111</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="10">
+        <v>840876</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="9">
+        <v>3</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="10">
+        <v>121</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
     <row r="28" spans="1:9" ht="18.75">
-      <c r="A28" s="12" t="s">
-        <v>14</v>
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1">
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30">
+      <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>2</v>
       </c>
@@ -793,61 +847,195 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="8">
-        <v>3090</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B30" s="8"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="6">
+        <v>12283750</v>
+      </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="10"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7">
+        <v>6326660</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7">
+        <v>4814980</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="10">
+        <v>1487991</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="10">
+        <v>71</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="18.75">
+      <c r="A36" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30">
+      <c r="B37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="8">
+        <v>3090</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6">
+        <f>B38</f>
+        <v>3090</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="9">
+        <v>20589</v>
+      </c>
+      <c r="D39">
+        <f>B39</f>
+        <v>20589</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="5"/>
+      <c r="B40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="18.75">
+      <c r="A44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30">
+      <c r="B46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="18.75">
-      <c r="A35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30">
-      <c r="B36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
+      <c r="B47">
+        <v>18324819</v>
+      </c>
+      <c r="D47">
+        <v>19241248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
         <v>16</v>
       </c>
-      <c r="B37">
+      <c r="B48">
         <v>18324819</v>
       </c>
-      <c r="D37">
-        <v>19241248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38">
-        <v>18324819</v>
-      </c>
-      <c r="D38">
+      <c r="D48">
         <v>8215824</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimizations returned, updated report
</commit_message>
<xml_diff>
--- a/Report/PR3 Measurements.xlsx
+++ b/Report/PR3 Measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>Measurements for PR3 Final Assignment</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Smoke::Tick is per instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Results aren't 100% accurate but are decent indications</t>
+  </si>
+  <si>
+    <t>Averaging out the results gives measurement errors, in DrawTanks for example</t>
   </si>
 </sst>
 </file>
@@ -486,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,11 +517,17 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>20</v>
       </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="18.75">
       <c r="A4" s="1" t="s">
@@ -544,7 +556,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="8">
-        <v>94738</v>
+        <v>88104</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6">
@@ -560,7 +572,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="9">
-        <v>106594007</v>
+        <v>95998558</v>
       </c>
       <c r="D7">
         <v>542734</v>
@@ -575,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="9">
-        <v>106416587</v>
+        <v>95837864</v>
       </c>
       <c r="D8">
         <v>356782</v>
@@ -590,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="9">
-        <v>151212</v>
+        <v>162579</v>
       </c>
       <c r="D9">
         <v>159214</v>
@@ -642,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="8">
-        <v>281584</v>
+        <v>307184</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6">
@@ -659,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="9">
-        <v>190303329</v>
+        <v>191395432</v>
       </c>
       <c r="D15" s="10">
         <v>1035457</v>
@@ -675,7 +687,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="9">
-        <v>190003775</v>
+        <v>191121105</v>
       </c>
       <c r="D16" s="10">
         <v>690674</v>
@@ -691,7 +703,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="9">
-        <v>274187</v>
+        <v>340570</v>
       </c>
       <c r="D17" s="10">
         <v>320689</v>
@@ -707,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="9">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D18" s="10">
         <v>167</v>
@@ -744,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="8">
-        <v>3814491</v>
+        <v>4666242</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6">
@@ -760,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="9">
-        <v>606472930</v>
+        <v>699634715</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7">
@@ -776,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="9">
-        <v>606076953</v>
+        <v>699763880</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7">
@@ -792,7 +804,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="9">
-        <v>371111</v>
+        <v>1066045</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="10">
@@ -849,7 +861,9 @@
       <c r="A30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="8">
+        <v>17914301</v>
+      </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>12283750</v>
@@ -863,7 +877,9 @@
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="9">
+        <v>1384320501</v>
+      </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7">
         <v>6326660</v>
@@ -877,7 +893,9 @@
       <c r="A32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="9"/>
+      <c r="B32" s="9">
+        <v>138525268</v>
+      </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7">
         <v>4814980</v>
@@ -891,7 +909,9 @@
       <c r="A33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="9">
+        <v>1558078</v>
+      </c>
       <c r="C33" s="7"/>
       <c r="D33" s="10">
         <v>1487991</v>
@@ -905,7 +925,9 @@
       <c r="A34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
       <c r="C34" s="7"/>
       <c r="D34" s="10">
         <v>71</v>

</xml_diff>